<commit_message>
Fix: bugs in data.xlsx
</commit_message>
<xml_diff>
--- a/Forum.Data/data/data.xlsx
+++ b/Forum.Data/data/data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Cloud\GitHub\Workshop_Forum\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Cloud\GitHub\Workshop_Forum\Forum.Data\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="categories" sheetId="4" r:id="rId1"/>
@@ -110,9 +110,6 @@
     <t>The domestic cat is believed to have evolved from the Near Eastern wildcat, whose range covers vast portions of the Middle East westward to the Atlantic coast of Africa.</t>
   </si>
   <si>
-    <t>The origin of the English word cat (Old English catt) and its counterparts in other Germanic languages (such as German Katze), descended from Proto-Germanic *kattōn-, is controversial. </t>
-  </si>
-  <si>
     <t>What is a cat?</t>
   </si>
   <si>
@@ -168,6 +165,9 @@
   </si>
   <si>
     <t>7,8,10</t>
+  </si>
+  <si>
+    <t>The origin of the English word cat (Old English catt) and its counterparts in other Germanic languages (such as German Katze), descended from Proto-Germanic *katton, is controversial.</t>
   </si>
 </sst>
 </file>
@@ -506,7 +506,7 @@
         <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -517,7 +517,7 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -528,7 +528,7 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -574,7 +574,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -602,7 +602,7 @@
         <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -616,7 +616,7 @@
         <v>9</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -628,14 +628,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="25.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="54.140625" customWidth="1"/>
     <col min="4" max="4" width="5.5703125" customWidth="1"/>
     <col min="5" max="5" width="7.7109375" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="1"/>
@@ -718,7 +718,7 @@
         <v>4</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -755,7 +755,7 @@
         <v>2</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -775,7 +775,7 @@
         <v>3</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -783,10 +783,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -808,13 +808,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="39.5703125" customWidth="1"/>
+    <col min="2" max="2" width="67.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -822,7 +822,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C1">
         <v>1</v>
@@ -836,7 +836,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -850,7 +850,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -864,7 +864,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -878,7 +878,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -892,7 +892,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -906,7 +906,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -920,7 +920,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8">
         <v>3</v>
@@ -934,7 +934,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -948,7 +948,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -962,7 +962,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C11">
         <v>3</v>

</xml_diff>